<commit_message>
Updated all data files.
</commit_message>
<xml_diff>
--- a/data/model/nBerkovich_r_linear.xlsx
+++ b/data/model/nBerkovich_r_linear.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josep\GitHub\NN_TiAlTa\data\model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{693F035B-4375-4460-AEE6-FFCF241A3B80}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB92CDBF-FE42-4FB1-8E62-050B3535379C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="495" windowWidth="28800" windowHeight="13620" xr2:uid="{22A46240-1FAA-4683-91B8-CDEDEB32A322}"/>
   </bookViews>
@@ -392,8 +392,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1830E8A8-A2DA-40CF-AFFA-FCF2BEB6AEEF}">
   <dimension ref="A1:DT159"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="CV1" workbookViewId="0">
-      <selection activeCell="DB9" sqref="DB9"/>
+    <sheetView tabSelected="1" topLeftCell="DI1" workbookViewId="0">
+      <selection activeCell="DV7" sqref="DV7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>